<commit_message>
Fixed error in high current mx fab BOM.
</commit_message>
<xml_diff>
--- a/hardware/pcbs/itsy_bitsy_mx_shield_v0p1/high_current/gerber_v0p1_r3/fab_files/RSTAT_MX_HC_BOM_JLCPCB.xlsx
+++ b/hardware/pcbs/itsy_bitsy_mx_shield_v0p1/high_current/gerber_v0p1_r3/fab_files/RSTAT_MX_HC_BOM_JLCPCB.xlsx
@@ -209,40 +209,40 @@
     <t xml:space="preserve">C25803</t>
   </si>
   <si>
-    <t xml:space="preserve">300k Resistor, 1%</t>
+    <t xml:space="preserve">30k Resistor, 1%</t>
   </si>
   <si>
     <t xml:space="preserve">R14</t>
   </si>
   <si>
-    <t xml:space="preserve">C23024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30k Resistor, 1%</t>
+    <t xml:space="preserve">C22984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3k Resistor, 1%</t>
   </si>
   <si>
     <t xml:space="preserve">R15</t>
   </si>
   <si>
-    <t xml:space="preserve">C22984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3k Resistor, 1%</t>
+    <t xml:space="preserve">C4211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 Ohm Resistor, 1%</t>
   </si>
   <si>
     <t xml:space="preserve">R16</t>
   </si>
   <si>
-    <t xml:space="preserve">C4211</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300 Ohm Resistor, 1%</t>
+    <t xml:space="preserve">C23025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.1 Ohm Resistor, 1%, 200mW</t>
   </si>
   <si>
     <t xml:space="preserve">R17</t>
   </si>
   <si>
-    <t xml:space="preserve">C23025</t>
+    <t xml:space="preserve"> C365143</t>
   </si>
   <si>
     <t xml:space="preserve">2k Resistor, 1%</t>
@@ -560,7 +560,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -891,9 +891,6 @@
       </c>
       <c r="D19" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="E19" s="4" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="20" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>